<commit_message>
Mejora en la auditoria de modelos ET
</commit_message>
<xml_diff>
--- a/BimManagement/BimManagement/Commands/ModelAudit/Config/audit format.xlsx
+++ b/BimManagement/BimManagement/Commands/ModelAudit/Config/audit format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Autodesk\Revit\Addins\2024\CESEL\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\cesel-audit-models\BimManagement\BimManagement\Commands\ModelAudit\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF51B0B0-745E-4120-8385-CFD7F73D6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066ECE4F-B224-42F2-A0E6-4DC1C466F618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auditoria" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   <definedNames>
     <definedName name="entregable">[1]INICIAL!$E$11</definedName>
     <definedName name="fecha">[1]INICIAL!$E$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Auditoria!$1:$8</definedName>
     <definedName name="responsable">[1]INICIAL!$E$13</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Auditoria!$1:$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>-</t>
   </si>
@@ -340,6 +340,9 @@
  = N° total de ítems establecidos de evaluación.  
 Cumplimiento de la Auditoría de Calidad (%)     
 2* En el caso que algun criterio no aplique, este se resta en el computo y/o calculo del % de cumplimiento de la auditoria de calidad.</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -588,6 +591,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -600,12 +612,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -614,49 +620,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -757,6 +727,39 @@
           <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1025,7 +1028,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DESCRIPCION DEL_x000a_PUNTO A EVALUAR" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="2235055-CPA-UT3-B02-ZZZ-M3D-SSA-AulasOficinas" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="COMENTARIO_x000a_DE LA REVISION" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="COMENTARIO_x000a_DE LA REVISION" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1297,28 +1300,28 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="6.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="18" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="67.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="67.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="22" style="3" customWidth="1"/>
     <col min="6" max="6" width="28" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="6.73046875" style="3"/>
+    <col min="7" max="16384" width="6.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="24" t="s">
+    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="27" t="s">
         <v>90</v>
       </c>
       <c r="E1" s="19" t="s">
@@ -1328,11 +1331,11 @@
         <v>240800</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="24"/>
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="19" t="s">
         <v>84</v>
       </c>
@@ -1340,10 +1343,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
@@ -1354,13 +1357,13 @@
         <v>45664</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="22" t="s">
         <v>86</v>
       </c>
@@ -1368,13 +1371,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
@@ -1383,13 +1386,13 @@
         <v>2235055-CPA-UT3-B02-ZZZ-M3D-SSA-AulasOficinas</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -1401,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39.4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -1421,11 +1424,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28">
+    <row r="9" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
         <v>1</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1434,74 +1437,86 @@
       <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
+    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
+    <row r="14" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28">
+    <row r="15" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
         <v>2</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1510,86 +1525,100 @@
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="33"/>
+    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="33"/>
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="33"/>
+    <row r="18" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="33"/>
+    <row r="19" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="33"/>
+    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="33"/>
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="14"/>
+      <c r="E21" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="28">
+    <row r="22" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
         <v>3</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -1598,38 +1627,44 @@
       <c r="D22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
+    <row r="23" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="28">
+    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
         <v>4</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="33" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="16" t="s">
@@ -1638,30 +1673,31 @@
       <c r="D25" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="32"/>
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="16" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="14" t="str">
-        <f>IF(E25="","",E25)</f>
-        <v/>
+      <c r="E26" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F26" s="15" t="str">
         <f>IF(F25="","",F25)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="32"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="16" t="s">
         <v>52</v>
       </c>
@@ -1673,11 +1709,11 @@
       </c>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="28">
+    <row r="28" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
         <v>5</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -1686,24 +1722,28 @@
       <c r="D28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="14"/>
+      <c r="E28" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
+    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="14"/>
+      <c r="E29" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
+    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="12" t="s">
         <v>60</v>
       </c>
@@ -1715,11 +1755,11 @@
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.35">
-      <c r="A31" s="28">
+    <row r="31" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
         <v>6</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="24" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -1728,38 +1768,44 @@
       <c r="D31" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
+    <row r="32" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="14"/>
+      <c r="E32" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F32" s="15"/>
     </row>
-    <row r="33" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="14"/>
+      <c r="E33" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F33" s="15"/>
     </row>
-    <row r="34" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28">
+    <row r="34" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25">
         <v>7</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -1768,26 +1814,30 @@
       <c r="D34" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="14"/>
+      <c r="E34" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F34" s="15"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
+    <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="14"/>
+      <c r="E35" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="28">
+    <row r="36" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
         <v>8</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="24" t="s">
         <v>74</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -1796,76 +1846,84 @@
       <c r="D36" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="14"/>
+      <c r="E36" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
+    <row r="37" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="16" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="14"/>
+      <c r="E37" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F37" s="15"/>
     </row>
-    <row r="38" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="29"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="12" t="s">
         <v>79</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="14"/>
+      <c r="E38" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F38" s="15"/>
     </row>
-    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
+    <row r="39" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="14"/>
+      <c r="E39" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F39" s="15"/>
     </row>
-    <row r="40" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="25" t="s">
+    <row r="40" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="17" t="str">
+      <c r="E40" s="17">
         <f>+IFERROR(+(COUNTIF(E$9:E$39,"SI")/(COUNTIF(E$9:E$39,"SI")+COUNTIF(E$9:E$39,"NO"))),"-")</f>
-        <v>-</v>
+        <v>1</v>
       </c>
       <c r="F40" s="5" t="str">
         <f>+IF(E40="-","-",IF(E40&lt;60.1%,"CONFIABILIDAD BAJA",IF(E40&lt;85.1%,"CONFIABILIDAD MEDIA",IF(E40&lt;100.1%,"CONFIABILIDAD ALTA",""))))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+        <v>CONFIABILIDAD ALTA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
@@ -1873,11 +1931,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A34:A35"/>
@@ -1894,45 +1947,50 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E39">
-    <cfRule type="cellIs" dxfId="11" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="113" operator="equal">
       <formula>"NO APLICA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="114" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="115" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="116" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="7" priority="238" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="238" operator="lessThan">
       <formula>0.601</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="240" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="240" operator="lessThan">
       <formula>0.851</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="242" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="242" operator="lessThan">
       <formula>1.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:F40">
-    <cfRule type="cellIs" dxfId="4" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="237" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="cellIs" dxfId="3" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="239" operator="equal">
       <formula>"CONFIABILIDAD BAJA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="241" operator="equal">
       <formula>"CONFIABILIDAD MEDIA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="243" operator="equal">
       <formula>"CONFIABILIDAD ALTA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1947,6 +2005,66 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Refrencia xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Refrencia>
+    <HTD_x0020_recepcion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <k66838accd504e12bd75da04acc36cb8 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ORGANIZACION INTERNACIONAL PARA LAS MIGRACIONES</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bcfa6c14-62f0-4329-801a-2463aa589465</TermId>
+        </TermInfo>
+      </Terms>
+    </k66838accd504e12bd75da04acc36cb8>
+    <Asunto xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <Remitente xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <General4 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <Adjunto xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Adjunto>
+    <a1609b5a0b5f46c3bf9a39af537e25e0 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Supervisión Escuela de Oficiales PNP Chorrillos</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bdf6216b-9251-4218-a718-efee418e2107</TermId>
+        </TermInfo>
+      </Terms>
+    </a1609b5a0b5f46c3bf9a39af537e25e0>
+    <Fecha_x0020_de_x0020_transmision xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <General2 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <Fecha_x0020_de_x0020_recepcion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Value>93</Value>
+      <Value>92</Value>
+      <Value>85</Value>
+    </TaxCatchAll>
+    <TipoDeDocumento xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <Atencion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <HTD_x0020_envio xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <FlujoAprobacion xmlns="07a04526-e23d-43a9-9176-684526d0d7d7">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </FlujoAprobacion>
+    <General3 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+    <l6a7d041aa9c4b9ca764daaaeb583fb6 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">240800</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d81ca66-ed94-4edb-8c9f-3ba0303a6a35</TermId>
+        </TermInfo>
+      </Terms>
+    </l6a7d041aa9c4b9ca764daaaeb583fb6>
+    <General1 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TC primario" ma:contentTypeID="0x010100715D56E80292094587AC535CEB94BB95006372F71B00ABE14187E0EACAE5BAD46B" ma:contentTypeVersion="41" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5965b7c11f53a64e9a1b1251209e7585">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xmlns:ns3="07a04526-e23d-43a9-9176-684526d0d7d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef4485d1477feebcf8d6c6977b6d41f6" ns1:_="" ns3:_="">
     <xsd:import namespace="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4"/>
@@ -2269,67 +2387,12 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Refrencia xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Refrencia>
-    <HTD_x0020_recepcion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <k66838accd504e12bd75da04acc36cb8 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ORGANIZACION INTERNACIONAL PARA LAS MIGRACIONES</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bcfa6c14-62f0-4329-801a-2463aa589465</TermId>
-        </TermInfo>
-      </Terms>
-    </k66838accd504e12bd75da04acc36cb8>
-    <Asunto xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <Remitente xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <General4 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <Adjunto xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Adjunto>
-    <a1609b5a0b5f46c3bf9a39af537e25e0 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Supervisión Escuela de Oficiales PNP Chorrillos</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bdf6216b-9251-4218-a718-efee418e2107</TermId>
-        </TermInfo>
-      </Terms>
-    </a1609b5a0b5f46c3bf9a39af537e25e0>
-    <Fecha_x0020_de_x0020_transmision xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <General2 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <Fecha_x0020_de_x0020_recepcion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Value>93</Value>
-      <Value>92</Value>
-      <Value>85</Value>
-    </TaxCatchAll>
-    <TipoDeDocumento xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <Atencion xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <HTD_x0020_envio xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <FlujoAprobacion xmlns="07a04526-e23d-43a9-9176-684526d0d7d7">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </FlujoAprobacion>
-    <General3 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-    <l6a7d041aa9c4b9ca764daaaeb583fb6 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">240800</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d81ca66-ed94-4edb-8c9f-3ba0303a6a35</TermId>
-        </TermInfo>
-      </Terms>
-    </l6a7d041aa9c4b9ca764daaaeb583fb6>
-    <General1 xmlns="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2338,12 +2401,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11719D67-3FF6-4B99-A0BA-B8DB81E4505B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="07a04526-e23d-43a9-9176-684526d0d7d7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AC1F934-9BBF-4284-B8EF-17F24E6895D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2362,35 +2437,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11719D67-3FF6-4B99-A0BA-B8DB81E4505B}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5842BE52-E846-4139-9C5A-1E63C941DA24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="07a04526-e23d-43a9-9176-684526d0d7d7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a9b2221c-e067-4b8a-9bf9-83fdb561d5d4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B65981A-96D5-4BD1-BAF9-5CA2E2FF7E84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5842BE52-E846-4139-9C5A-1E63C941DA24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>